<commit_message>
Android now supports background images
</commit_message>
<xml_diff>
--- a/CurrentFeatures.xlsx
+++ b/CurrentFeatures.xlsx
@@ -6,37 +6,18 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Export Summary" sheetId="1" r:id="rId4"/>
-    <sheet name="Sheet 1 - Features" sheetId="2" r:id="rId5"/>
-    <sheet name="Sheet 1 - Image export" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet 1 - Features" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1 - Image export" sheetId="2" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
-  <si>
-    <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
-  </si>
-  <si>
-    <t>Numbers Sheet Name</t>
-  </si>
-  <si>
-    <t>Numbers Table Name</t>
-  </si>
-  <si>
-    <t>Excel Worksheet Name</t>
-  </si>
-  <si>
-    <t>Sheet 1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
   <si>
     <t>Features</t>
   </si>
   <si>
-    <t>Sheet 1 - Features</t>
-  </si>
-  <si>
     <t>iOS</t>
   </si>
   <si>
@@ -128,9 +109,6 @@
   </si>
   <si>
     <t>Zoom/Scaling</t>
-  </si>
-  <si>
-    <t>Sheet 1 - Image export</t>
   </si>
   <si>
     <t>Image</t>
@@ -167,17 +145,16 @@
     <font>
       <sz val="12"/>
       <color indexed="8"/>
-      <name val="Helvetica"/>
+      <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="14"/>
+      <sz val="13"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
     </font>
     <font>
-      <u val="single"/>
       <sz val="12"/>
-      <color indexed="11"/>
+      <color indexed="8"/>
       <name val="Helvetica"/>
     </font>
     <font>
@@ -202,13 +179,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
+        <fgColor indexed="12"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="12"/>
+        <fgColor indexed="14"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -249,7 +226,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -259,7 +236,59 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
         <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="13"/>
@@ -268,7 +297,7 @@
         <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="14"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -277,28 +306,43 @@
         <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="14"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="14"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="14"/>
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="14"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -307,58 +351,63 @@
         <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="14"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="14"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="14"/>
-      </left>
+      <left/>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -368,96 +417,107 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -477,11 +537,10 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="015e88b1"/>
-      <rgbColor rgb="01eef3f4"/>
-      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ffffe061"/>
@@ -489,6 +548,7 @@
       <rgbColor rgb="fffefefe"/>
       <rgbColor rgb="ffff2c21"/>
       <rgbColor rgb="ffffa93a"/>
+      <rgbColor rgb="ff6ec038"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -505,10 +565,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="404040"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="BFBFBF"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="499BC9"/>
@@ -537,14 +597,14 @@
     </a:clrScheme>
     <a:fontScheme name="Blank">
       <a:majorFont>
-        <a:latin typeface="Helvetica"/>
-        <a:ea typeface="Helvetica"/>
-        <a:cs typeface="Helvetica"/>
+        <a:latin typeface="Helvetica Neue"/>
+        <a:ea typeface="Helvetica Neue"/>
+        <a:cs typeface="Helvetica Neue"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Helvetica"/>
-        <a:ea typeface="Helvetica"/>
-        <a:cs typeface="Helvetica"/>
+        <a:latin typeface="Helvetica Neue"/>
+        <a:ea typeface="Helvetica Neue"/>
+        <a:cs typeface="Helvetica Neue"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Blank">
@@ -702,14 +762,15 @@
   <a:objectDefaults>
     <a:spDef>
       <a:spPr>
-        <a:blipFill rotWithShape="1">
-          <a:blip r:embed="rId1"/>
-          <a:srcRect l="0" t="0" r="0" b="0"/>
-          <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
-        </a:blipFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst>
           <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
@@ -724,39 +785,33 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:effectLst>
-              <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="25400" dist="23998" dir="2700000">
-                <a:srgbClr val="000000">
-                  <a:alpha val="31034"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-            <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Helvetica"/>
+            <a:ea typeface="Helvetica"/>
+            <a:cs typeface="Helvetica"/>
             <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
@@ -1005,14 +1060,20 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="6350" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
-        <a:effectLst/>
+        <a:effectLst>
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:srgbClr val="000000">
+              <a:alpha val="50000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -1301,7 +1362,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1325,9 +1386,9 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
+            <a:latin typeface="Helvetica"/>
+            <a:ea typeface="Helvetica"/>
+            <a:cs typeface="Helvetica"/>
             <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
@@ -1579,66 +1640,299 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="4" width="33.6016" customWidth="1"/>
+    <col min="1" max="1" width="26.8516" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.3516" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.3516" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.3516" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.3516" style="1" customWidth="1"/>
+    <col min="6" max="256" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" ht="50" customHeight="1">
-      <c r="B3" t="s" s="1">
+    <row r="1" ht="28" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="C3"/>
-      <c r="D3"/>
-    </row>
-    <row r="7">
-      <c r="B7" t="s" s="2">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" ht="20.55" customHeight="1">
+      <c r="A2" s="5"/>
+      <c r="B2" t="s" s="6">
         <v>1</v>
       </c>
-      <c r="C7" t="s" s="2">
+      <c r="C2" t="s" s="6">
         <v>2</v>
       </c>
-      <c r="D7" t="s" s="2">
+      <c r="D2" t="s" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="B9" t="s" s="3">
+      <c r="E2" t="s" s="6">
         <v>4</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10">
-      <c r="B10" s="4"/>
-      <c r="C10" t="s" s="4">
+    </row>
+    <row r="3" ht="20.55" customHeight="1">
+      <c r="A3" t="s" s="7">
         <v>5</v>
       </c>
-      <c r="D10" t="s" s="5">
+      <c r="B3" s="8"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" ht="20.35" customHeight="1">
+      <c r="A4" t="s" s="10">
         <v>6</v>
       </c>
-    </row>
-    <row r="11">
-      <c r="B11" s="4"/>
-      <c r="C11" t="s" s="4">
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+    </row>
+    <row r="5" ht="20.35" customHeight="1">
+      <c r="A5" t="s" s="10">
+        <v>7</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+    </row>
+    <row r="6" ht="20.35" customHeight="1">
+      <c r="A6" t="s" s="10">
+        <v>8</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+    </row>
+    <row r="7" ht="20.35" customHeight="1">
+      <c r="A7" t="s" s="10">
+        <v>9</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" ht="32.35" customHeight="1">
+      <c r="A8" t="s" s="10">
+        <v>10</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="12"/>
+      <c r="D8" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="E8" s="14"/>
+    </row>
+    <row r="9" ht="20.35" customHeight="1">
+      <c r="A9" t="s" s="10">
+        <v>12</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="14"/>
+    </row>
+    <row r="10" ht="20.35" customHeight="1">
+      <c r="A10" t="s" s="10">
+        <v>13</v>
+      </c>
+      <c r="B10" s="15"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+    </row>
+    <row r="11" ht="20.35" customHeight="1">
+      <c r="A11" t="s" s="10">
+        <v>14</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+    </row>
+    <row r="12" ht="20.35" customHeight="1">
+      <c r="A12" t="s" s="10">
+        <v>15</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+    </row>
+    <row r="13" ht="20.35" customHeight="1">
+      <c r="A13" t="s" s="10">
+        <v>16</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+    </row>
+    <row r="14" ht="44.35" customHeight="1">
+      <c r="A14" t="s" s="10">
+        <v>17</v>
+      </c>
+      <c r="B14" s="19"/>
+      <c r="C14" s="16"/>
+      <c r="D14" t="s" s="13">
+        <v>18</v>
+      </c>
+      <c r="E14" s="20"/>
+    </row>
+    <row r="15" ht="20.35" customHeight="1">
+      <c r="A15" s="10"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="20"/>
+    </row>
+    <row r="16" ht="20.35" customHeight="1">
+      <c r="A16" t="s" s="10">
         <v>19</v>
       </c>
-      <c r="D11" t="s" s="5">
-        <v>38</v>
-      </c>
+      <c r="B16" s="23"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+    </row>
+    <row r="17" ht="20.35" customHeight="1">
+      <c r="A17" t="s" s="10">
+        <v>20</v>
+      </c>
+      <c r="B17" s="15"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+    </row>
+    <row r="18" ht="20.35" customHeight="1">
+      <c r="A18" t="s" s="10">
+        <v>21</v>
+      </c>
+      <c r="B18" s="15"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+    </row>
+    <row r="19" ht="20.35" customHeight="1">
+      <c r="A19" t="s" s="10">
+        <v>22</v>
+      </c>
+      <c r="B19" s="19"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+    </row>
+    <row r="20" ht="32.35" customHeight="1">
+      <c r="A20" t="s" s="10">
+        <v>23</v>
+      </c>
+      <c r="B20" s="15"/>
+      <c r="C20" s="17"/>
+      <c r="D20" t="s" s="25">
+        <v>24</v>
+      </c>
+      <c r="E20" s="17"/>
+    </row>
+    <row r="21" ht="20.35" customHeight="1">
+      <c r="A21" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="B21" s="15"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+    </row>
+    <row r="22" ht="20.35" customHeight="1">
+      <c r="A22" s="26"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+    </row>
+    <row r="23" ht="20.35" customHeight="1">
+      <c r="A23" t="s" s="10">
+        <v>26</v>
+      </c>
+      <c r="B23" s="23"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+    </row>
+    <row r="24" ht="20.35" customHeight="1">
+      <c r="A24" t="s" s="10">
+        <v>27</v>
+      </c>
+      <c r="B24" s="15"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+    </row>
+    <row r="25" ht="20.35" customHeight="1">
+      <c r="A25" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="B25" s="15"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+    </row>
+    <row r="26" ht="20.35" customHeight="1">
+      <c r="A26" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="B26" s="15"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+    </row>
+    <row r="27" ht="20.35" customHeight="1">
+      <c r="A27" t="s" s="10">
+        <v>30</v>
+      </c>
+      <c r="B27" s="15"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+    </row>
+    <row r="28" ht="20.35" customHeight="1">
+      <c r="A28" t="s" s="10">
+        <v>31</v>
+      </c>
+      <c r="B28" s="15"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+    </row>
+    <row r="29" ht="20.35" customHeight="1">
+      <c r="A29" s="10"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="D10" location="'Sheet 1 - Features'!R2C1" tooltip="" display="Sheet 1 - Features"/>
-    <hyperlink ref="D11" location="'Sheet 1 - Image export'!R2C1" tooltip="" display="Sheet 1 - Image export"/>
-  </hyperlinks>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1647,408 +1941,118 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:E29"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="26.7422" style="6" customWidth="1"/>
-    <col min="2" max="2" width="16.3516" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.3516" style="6" customWidth="1"/>
-    <col min="4" max="4" width="16.3516" style="6" customWidth="1"/>
-    <col min="5" max="5" width="16.3516" style="6" customWidth="1"/>
-    <col min="6" max="256" width="16.3516" style="6" customWidth="1"/>
+    <col min="1" max="1" width="20.6719" style="27" customWidth="1"/>
+    <col min="2" max="2" width="16.3516" style="27" customWidth="1"/>
+    <col min="3" max="3" width="16.3516" style="27" customWidth="1"/>
+    <col min="4" max="4" width="16.3516" style="27" customWidth="1"/>
+    <col min="5" max="5" width="16.3516" style="27" customWidth="1"/>
+    <col min="6" max="256" width="16.3516" style="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="28" customHeight="1">
-      <c r="A1" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="A1" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="28"/>
     </row>
     <row r="2" ht="20.55" customHeight="1">
-      <c r="A2" s="8"/>
-      <c r="B2" t="s" s="9">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s" s="9">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s" s="9">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s" s="9">
-        <v>10</v>
-      </c>
+      <c r="A2" s="5"/>
+      <c r="B2" t="s" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s" s="6">
+        <v>3</v>
+      </c>
+      <c r="E2" s="29"/>
     </row>
     <row r="3" ht="20.55" customHeight="1">
-      <c r="A3" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-    </row>
-    <row r="4" ht="20.35" customHeight="1">
-      <c r="A4" t="s" s="13">
-        <v>12</v>
-      </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-    </row>
-    <row r="5" ht="20.35" customHeight="1">
-      <c r="A5" t="s" s="13">
-        <v>13</v>
-      </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-    </row>
-    <row r="6" ht="20.35" customHeight="1">
-      <c r="A6" t="s" s="13">
-        <v>14</v>
-      </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-    </row>
-    <row r="7" ht="20.35" customHeight="1">
-      <c r="A7" t="s" s="13">
-        <v>15</v>
-      </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-    </row>
-    <row r="8" ht="32.35" customHeight="1">
-      <c r="A8" t="s" s="13">
-        <v>16</v>
-      </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="15"/>
-      <c r="D8" t="s" s="16">
-        <v>17</v>
-      </c>
-      <c r="E8" s="17"/>
-    </row>
-    <row r="9" ht="20.35" customHeight="1">
-      <c r="A9" t="s" s="13">
-        <v>18</v>
-      </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="17"/>
-    </row>
-    <row r="10" ht="20.35" customHeight="1">
-      <c r="A10" t="s" s="13">
-        <v>19</v>
-      </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-    </row>
-    <row r="11" ht="20.35" customHeight="1">
-      <c r="A11" t="s" s="13">
-        <v>20</v>
-      </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-    </row>
-    <row r="12" ht="20.35" customHeight="1">
-      <c r="A12" t="s" s="13">
-        <v>21</v>
-      </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-    </row>
-    <row r="13" ht="20.35" customHeight="1">
-      <c r="A13" t="s" s="13">
-        <v>22</v>
-      </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-    </row>
-    <row r="14" ht="44.35" customHeight="1">
-      <c r="A14" t="s" s="13">
-        <v>23</v>
-      </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="21"/>
-      <c r="D14" t="s" s="16">
-        <v>24</v>
-      </c>
-      <c r="E14" s="22"/>
-    </row>
-    <row r="15" ht="20.35" customHeight="1">
-      <c r="A15" s="13"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="22"/>
-    </row>
-    <row r="16" ht="20.35" customHeight="1">
-      <c r="A16" t="s" s="13">
-        <v>25</v>
-      </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-    </row>
-    <row r="17" ht="20.35" customHeight="1">
-      <c r="A17" t="s" s="13">
-        <v>26</v>
-      </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-    </row>
-    <row r="18" ht="20.35" customHeight="1">
-      <c r="A18" t="s" s="13">
-        <v>27</v>
-      </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-    </row>
-    <row r="19" ht="20.35" customHeight="1">
-      <c r="A19" t="s" s="13">
-        <v>28</v>
-      </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-    </row>
-    <row r="20" ht="32.35" customHeight="1">
-      <c r="A20" t="s" s="13">
-        <v>29</v>
-      </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="19"/>
-      <c r="D20" t="s" s="27">
-        <v>30</v>
-      </c>
-      <c r="E20" s="19"/>
-    </row>
-    <row r="21" ht="20.35" customHeight="1">
-      <c r="A21" t="s" s="13">
-        <v>31</v>
-      </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-    </row>
-    <row r="22" ht="20.35" customHeight="1">
-      <c r="A22" s="28"/>
-      <c r="B22" s="23"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-    </row>
-    <row r="23" ht="20.35" customHeight="1">
-      <c r="A23" t="s" s="13">
+      <c r="A3" t="s" s="7">
         <v>32</v>
-      </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-    </row>
-    <row r="24" ht="20.35" customHeight="1">
-      <c r="A24" t="s" s="13">
-        <v>33</v>
-      </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-    </row>
-    <row r="25" ht="20.35" customHeight="1">
-      <c r="A25" t="s" s="13">
-        <v>34</v>
-      </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-    </row>
-    <row r="26" ht="20.35" customHeight="1">
-      <c r="A26" t="s" s="13">
-        <v>35</v>
-      </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-    </row>
-    <row r="27" ht="20.35" customHeight="1">
-      <c r="A27" t="s" s="13">
-        <v>36</v>
-      </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-    </row>
-    <row r="28" ht="20.35" customHeight="1">
-      <c r="A28" t="s" s="13">
-        <v>37</v>
-      </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-    </row>
-    <row r="29" ht="20.35" customHeight="1">
-      <c r="A29" s="13"/>
-      <c r="B29" s="23"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
-  </mergeCells>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A2:D11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col min="1" max="1" width="20.6094" style="29" customWidth="1"/>
-    <col min="2" max="2" width="16.3516" style="29" customWidth="1"/>
-    <col min="3" max="3" width="16.3516" style="29" customWidth="1"/>
-    <col min="4" max="4" width="16.3516" style="29" customWidth="1"/>
-    <col min="5" max="256" width="16.3516" style="29" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="28" customHeight="1">
-      <c r="A1" t="s" s="7">
-        <v>19</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-    </row>
-    <row r="2" ht="20.55" customHeight="1">
-      <c r="A2" s="8"/>
-      <c r="B2" t="s" s="9">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s" s="9">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s" s="9">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" ht="20.55" customHeight="1">
-      <c r="A3" t="s" s="10">
-        <v>39</v>
       </c>
       <c r="B3" s="30"/>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
+      <c r="E3" s="29"/>
     </row>
     <row r="4" ht="20.35" customHeight="1">
-      <c r="A4" t="s" s="13">
-        <v>40</v>
-      </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
+      <c r="A4" t="s" s="10">
+        <v>33</v>
+      </c>
+      <c r="B4" s="15"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="29"/>
     </row>
     <row r="5" ht="20.35" customHeight="1">
-      <c r="A5" t="s" s="13">
-        <v>41</v>
-      </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
+      <c r="A5" t="s" s="10">
+        <v>34</v>
+      </c>
+      <c r="B5" s="15"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="29"/>
     </row>
     <row r="6" ht="20.35" customHeight="1">
-      <c r="A6" t="s" s="13">
-        <v>42</v>
-      </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
+      <c r="A6" t="s" s="10">
+        <v>35</v>
+      </c>
+      <c r="B6" s="15"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="29"/>
     </row>
     <row r="7" ht="20.35" customHeight="1">
-      <c r="A7" t="s" s="13">
-        <v>22</v>
-      </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
+      <c r="A7" t="s" s="10">
+        <v>16</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="29"/>
     </row>
     <row r="8" ht="20.35" customHeight="1">
-      <c r="A8" t="s" s="13">
-        <v>43</v>
-      </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
+      <c r="A8" t="s" s="10">
+        <v>36</v>
+      </c>
+      <c r="B8" s="15"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="29"/>
     </row>
     <row r="9" ht="20.35" customHeight="1">
-      <c r="A9" t="s" s="13">
-        <v>44</v>
-      </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
+      <c r="A9" t="s" s="10">
+        <v>37</v>
+      </c>
+      <c r="B9" s="15"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="29"/>
     </row>
     <row r="10" ht="20.35" customHeight="1">
-      <c r="A10" s="28"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="29"/>
     </row>
     <row r="11" ht="20.35" customHeight="1">
-      <c r="A11" s="28"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="32"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2057,7 +2061,7 @@
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removed UWP completely (backup is in the last commit before this one)
</commit_message>
<xml_diff>
--- a/CurrentFeatures.xlsx
+++ b/CurrentFeatures.xlsx
@@ -1,19 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr date1904="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zezioen\Documents\XamarinPainter\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1 - Features" sheetId="1" r:id="rId4"/>
-    <sheet name="Sheet 1 - Image export" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet 1 - Features" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1 - Image export" sheetId="2" r:id="rId2"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>Features</t>
   </si>
@@ -24,9 +31,6 @@
     <t>Android</t>
   </si>
   <si>
-    <t>UWP</t>
-  </si>
-  <si>
     <t>Forms</t>
   </si>
   <si>
@@ -48,9 +52,6 @@
     <t>Orientation changes</t>
   </si>
   <si>
-    <t>Different orientation default</t>
-  </si>
-  <si>
     <t>Transparant background</t>
   </si>
   <si>
@@ -69,9 +70,6 @@
     <t>Efficient rendering</t>
   </si>
   <si>
-    <t>It’s a default class from Microsoft, go figure</t>
-  </si>
-  <si>
     <t>V1.1</t>
   </si>
   <si>
@@ -85,9 +83,6 @@
   </si>
   <si>
     <t>Smooth lines</t>
-  </si>
-  <si>
-    <t>Default except for loading</t>
   </si>
   <si>
     <t>Undo</t>
@@ -132,23 +127,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Helvetica"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="13"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
     </font>
@@ -158,7 +140,7 @@
       <name val="Helvetica"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
@@ -413,112 +395,103 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+  <cellXfs count="31">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -528,34 +501,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
-      <rgbColor rgb="ffffe061"/>
-      <rgbColor rgb="ff6dc037"/>
-      <rgbColor rgb="fffefefe"/>
-      <rgbColor rgb="ffff2c21"/>
-      <rgbColor rgb="ffffa93a"/>
-      <rgbColor rgb="ff6ec038"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="FFFFE061"/>
+      <rgbColor rgb="FF6DC037"/>
+      <rgbColor rgb="FFFEFEFE"/>
+      <rgbColor rgb="FFFF2C21"/>
+      <rgbColor rgb="FFFFA93A"/>
+      <rgbColor rgb="FF6EC038"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -681,7 +705,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -690,7 +714,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -699,7 +723,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -773,7 +797,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="50000"/>
             </a:srgbClr>
@@ -781,7 +805,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -800,7 +824,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -830,7 +854,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -856,7 +880,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -882,7 +906,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -908,7 +932,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -934,7 +958,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -960,7 +984,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -986,7 +1010,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1012,7 +1036,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1038,7 +1062,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1051,9 +1075,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1068,7 +1098,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="50000"/>
             </a:srgbClr>
@@ -1076,7 +1106,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1095,7 +1125,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1121,7 +1151,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1147,7 +1177,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1173,7 +1203,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1199,7 +1229,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1225,7 +1255,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1251,7 +1281,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1277,7 +1307,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1303,7 +1333,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1329,7 +1359,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1342,9 +1372,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1358,7 +1394,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1377,7 +1413,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1407,7 +1443,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1433,7 +1469,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1459,7 +1495,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1485,7 +1521,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1511,7 +1547,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1537,7 +1573,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1563,7 +1599,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1589,7 +1625,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1615,7 +1651,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1628,308 +1664,276 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:IU29"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D1:D1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.36328125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.8516" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.3516" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.3516" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.3516" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.3516" style="1" customWidth="1"/>
-    <col min="6" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.81640625" style="1" customWidth="1"/>
+    <col min="2" max="255" width="16.36328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="28" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
-    </row>
-    <row r="2" ht="20.55" customHeight="1">
-      <c r="A2" s="5"/>
-      <c r="B2" t="s" s="6">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="30"/>
+    </row>
+    <row r="2" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s" s="6">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s" s="6">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s" s="6">
+    </row>
+    <row r="3" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" ht="20.55" customHeight="1">
-      <c r="A3" t="s" s="7">
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+    </row>
+    <row r="4" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-    </row>
-    <row r="4" ht="20.35" customHeight="1">
-      <c r="A4" t="s" s="10">
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+    </row>
+    <row r="5" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-    </row>
-    <row r="5" ht="20.35" customHeight="1">
-      <c r="A5" t="s" s="10">
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+    </row>
+    <row r="6" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-    </row>
-    <row r="6" ht="20.35" customHeight="1">
-      <c r="A6" t="s" s="10">
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+    </row>
+    <row r="7" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-    </row>
-    <row r="7" ht="20.35" customHeight="1">
-      <c r="A7" t="s" s="10">
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="1:4" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-    </row>
-    <row r="8" ht="32.35" customHeight="1">
-      <c r="A8" t="s" s="10">
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="10"/>
+    </row>
+    <row r="9" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="12"/>
-      <c r="D8" t="s" s="13">
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="10"/>
+    </row>
+    <row r="10" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="14"/>
-    </row>
-    <row r="9" ht="20.35" customHeight="1">
-      <c r="A9" t="s" s="10">
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="13"/>
+    </row>
+    <row r="11" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="14"/>
-    </row>
-    <row r="10" ht="20.35" customHeight="1">
-      <c r="A10" t="s" s="10">
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-    </row>
-    <row r="11" ht="20.35" customHeight="1">
-      <c r="A11" t="s" s="10">
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-    </row>
-    <row r="12" ht="20.35" customHeight="1">
-      <c r="A12" t="s" s="10">
+      <c r="B13" s="8"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="13"/>
+    </row>
+    <row r="14" spans="1:4" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-    </row>
-    <row r="13" ht="20.35" customHeight="1">
-      <c r="A13" t="s" s="10">
+      <c r="B14" s="15"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="16"/>
+    </row>
+    <row r="15" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="16"/>
+    </row>
+    <row r="16" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-    </row>
-    <row r="14" ht="44.35" customHeight="1">
-      <c r="A14" t="s" s="10">
+      <c r="B16" s="18"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+    </row>
+    <row r="17" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="16"/>
-      <c r="D14" t="s" s="13">
+      <c r="B17" s="11"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+    </row>
+    <row r="18" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="20"/>
-    </row>
-    <row r="15" ht="20.35" customHeight="1">
-      <c r="A15" s="10"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="20"/>
-    </row>
-    <row r="16" ht="20.35" customHeight="1">
-      <c r="A16" t="s" s="10">
+      <c r="B18" s="11"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+    </row>
+    <row r="19" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="23"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-    </row>
-    <row r="17" ht="20.35" customHeight="1">
-      <c r="A17" t="s" s="10">
+      <c r="B19" s="15"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+    </row>
+    <row r="20" spans="1:4" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-    </row>
-    <row r="18" ht="20.35" customHeight="1">
-      <c r="A18" t="s" s="10">
+      <c r="B20" s="11"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+    </row>
+    <row r="21" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-    </row>
-    <row r="19" ht="20.35" customHeight="1">
-      <c r="A19" t="s" s="10">
+      <c r="B21" s="11"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+    </row>
+    <row r="22" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="20"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+    </row>
+    <row r="23" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-    </row>
-    <row r="20" ht="32.35" customHeight="1">
-      <c r="A20" t="s" s="10">
+      <c r="B23" s="18"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+    </row>
+    <row r="24" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="17"/>
-      <c r="D20" t="s" s="25">
+      <c r="B24" s="11"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+    </row>
+    <row r="25" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="17"/>
-    </row>
-    <row r="21" ht="20.35" customHeight="1">
-      <c r="A21" t="s" s="10">
+      <c r="B25" s="11"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+    </row>
+    <row r="26" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="15"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-    </row>
-    <row r="22" ht="20.35" customHeight="1">
-      <c r="A22" s="26"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-    </row>
-    <row r="23" ht="20.35" customHeight="1">
-      <c r="A23" t="s" s="10">
+      <c r="B26" s="11"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+    </row>
+    <row r="27" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-    </row>
-    <row r="24" ht="20.35" customHeight="1">
-      <c r="A24" t="s" s="10">
+      <c r="B27" s="11"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+    </row>
+    <row r="28" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-    </row>
-    <row r="25" ht="20.35" customHeight="1">
-      <c r="A25" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-    </row>
-    <row r="26" ht="20.35" customHeight="1">
-      <c r="A26" t="s" s="10">
-        <v>29</v>
-      </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-    </row>
-    <row r="27" ht="20.35" customHeight="1">
-      <c r="A27" t="s" s="10">
-        <v>30</v>
-      </c>
-      <c r="B27" s="15"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-    </row>
-    <row r="28" ht="20.35" customHeight="1">
-      <c r="A28" t="s" s="10">
-        <v>31</v>
-      </c>
-      <c r="B28" s="15"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-    </row>
-    <row r="29" ht="20.35" customHeight="1">
-      <c r="A29" s="10"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+    </row>
+    <row r="29" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -1937,129 +1941,114 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:IU11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.36328125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6719" style="27" customWidth="1"/>
-    <col min="2" max="2" width="16.3516" style="27" customWidth="1"/>
-    <col min="3" max="3" width="16.3516" style="27" customWidth="1"/>
-    <col min="4" max="4" width="16.3516" style="27" customWidth="1"/>
-    <col min="5" max="5" width="16.3516" style="27" customWidth="1"/>
-    <col min="6" max="256" width="16.3516" style="27" customWidth="1"/>
+    <col min="1" max="1" width="20.6328125" style="21" customWidth="1"/>
+    <col min="2" max="255" width="16.36328125" style="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="28" customHeight="1">
-      <c r="A1" t="s" s="2">
-        <v>13</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="28"/>
-    </row>
-    <row r="2" ht="20.55" customHeight="1">
-      <c r="A2" s="5"/>
-      <c r="B2" t="s" s="6">
+    <row r="1" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="22"/>
+    </row>
+    <row r="2" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s" s="6">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s" s="6">
-        <v>3</v>
-      </c>
-      <c r="E2" s="29"/>
-    </row>
-    <row r="3" ht="20.55" customHeight="1">
-      <c r="A3" t="s" s="7">
+      <c r="D2" s="23"/>
+    </row>
+    <row r="3" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="23"/>
+    </row>
+    <row r="4" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="23"/>
+    </row>
+    <row r="5" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="23"/>
+    </row>
+    <row r="6" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="23"/>
+    </row>
+    <row r="7" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="23"/>
+    </row>
+    <row r="8" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="29"/>
-    </row>
-    <row r="4" ht="20.35" customHeight="1">
-      <c r="A4" t="s" s="10">
+      <c r="B8" s="11"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="23"/>
+    </row>
+    <row r="9" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="29"/>
-    </row>
-    <row r="5" ht="20.35" customHeight="1">
-      <c r="A5" t="s" s="10">
-        <v>34</v>
-      </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="29"/>
-    </row>
-    <row r="6" ht="20.35" customHeight="1">
-      <c r="A6" t="s" s="10">
-        <v>35</v>
-      </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="29"/>
-    </row>
-    <row r="7" ht="20.35" customHeight="1">
-      <c r="A7" t="s" s="10">
-        <v>16</v>
-      </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="29"/>
-    </row>
-    <row r="8" ht="20.35" customHeight="1">
-      <c r="A8" t="s" s="10">
-        <v>36</v>
-      </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="29"/>
-    </row>
-    <row r="9" ht="20.35" customHeight="1">
-      <c r="A9" t="s" s="10">
-        <v>37</v>
-      </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="29"/>
-    </row>
-    <row r="10" ht="20.35" customHeight="1">
-      <c r="A10" s="26"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="29"/>
-    </row>
-    <row r="11" ht="20.35" customHeight="1">
-      <c r="A11" s="26"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="33"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="23"/>
+    </row>
+    <row r="10" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="20"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="23"/>
+    </row>
+    <row r="11" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="20"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:C1"/>
   </mergeCells>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>